<commit_message>
v0.14.10.0 beta. Updates on users, roles, and query helpers.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20180103.xlsx
+++ b/AIWE Table Making Guideline v20180103.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="675" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common Tables" sheetId="1" r:id="rId1"/>
@@ -17,15 +17,16 @@
     <sheet name="TC-SQLS" sheetId="7" r:id="rId8"/>
     <sheet name="Misc" sheetId="4" r:id="rId9"/>
     <sheet name="Development Ideas" sheetId="10" r:id="rId10"/>
-    <sheet name="Updates Log legacy" sheetId="3" r:id="rId11"/>
-    <sheet name="DBUpdates legacy" sheetId="5" r:id="rId12"/>
+    <sheet name="Alternate User Tables" sheetId="13" r:id="rId11"/>
+    <sheet name="Updates Log legacy" sheetId="3" r:id="rId12"/>
+    <sheet name="DBUpdates legacy" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1159">
   <si>
     <t>No</t>
   </si>
@@ -5161,6 +5162,21 @@
 GroupByColumn31:AutoDirective31,GroupByColumn32:AutoDirective32,…=AQ-SQLS-3</t>
   </si>
   <si>
+    <t xml:space="preserve">Complete Example 1: [IntTypeColumn,IntTypeCondColumn|GE|Avg(TableNameA:WorkHours)|green]
+Means:
+- IntTypeColumn will be colored to green when IntTypeCondColumn value is greater than or equal to Avg(TableNameA:Hours)
+Complete Example 2:
+[StringTypeColumn|E|Boss Name|red]
+Means:
+- StringTypeColumn will be colored to red when StringTypeColumn value is equal to "Boss Name"
+CompExp Examples:
+  - aggregateNames + self keyword: 
+     Avg(TableA:WorkHours) or Min(OwnTable:TargetColumn:self+30) or Max(OtherTable:TargetColumn:512-15) 512 is cid no
+  - using date time data type with the correct format:
+     2/24/2017 00:14:00 or NOW + 50 or OwnTable:TargetColumn:self+30 or TableA:WorkHours:12-15 -&gt; 12 is cid no
+</t>
+  </si>
+  <si>
     <t>To set criteria for coloring cell which meet the ColoringCondition. The ColoringCondition has the following format:
 [ColumnName,ConditionColumnName|CompCode|CompExp|HTML Color]
 ColumnName = The column to be colored for coloring condition. ConditionColumnName = The column to be checked for coloring condition. If this part is not written, then ColumnName will be used to check for the coloring condition. ColumnName and ConditionColumnName must be of same data type.
@@ -5175,24 +5191,72 @@
 OptionalSelf can be put as self which indicates cid of itself with option (+) or (-) a positive number
  self must be accompanied by its own table and its own column
 For date time data type, the format must be M/d/yyyy HH:mm:ss according to MSDN document or using keyword NOW 
- or table value reference in the form of RefTableName:RefTableColumn:OptionalSelf+-PosNum
-HTML color = HTML color code in text. For example: red or blue
+ or table value reference in the form of RefTableName:RefTableColumn:OptionalSelf+-PosNum. The PosNum is a positive number representing seconds.
+HTML color = HTML (web) color code in text. For example: red or blue. Custom color such as #FF4433 is applicable for AIWE
 If multiple conditions are applied to a single column, the color of the first (left-most) condition to be met will be applied</t>
   </si>
   <si>
-    <t xml:space="preserve">Complete Example 1: [IntTypeColumn,IntTypeCondColumn|GE|Avg(TableNameA:WorkHours)|green]
-Means:
-- IntTypeColumn will be colored to green when IntTypeCondColumn value is greater than or equal to Avg(TableNameA:Hours)
-Complete Example 2:
-[StringTypeColumn|E|Boss Name|red]
-Means:
-- StringTypeColumn will be colored to red when StringTypeColumn value is equal to "Boss Name"
-CompExp Examples:
-  - aggregateNames + self keyword: 
-     Avg(TableA:WorkHours) or Min(OwnTable:TargetColumn:self+30) or Max(OtherTable:TargetColumn:512-15) 512 is cid no
-  - using date time data type with the correct format:
-     2/24/2017 00:14:00 or NOW + 50 or OwnTable:TargetColumn:self+30 or TableA:WorkHours:12-15 -&gt; 12 is cid no
-</t>
+    <t>create table Users (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Email nvarchar(500),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PasswordHash nvarchar(300),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  FullName nvarchar(300),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  DisplayName nvarchar(300),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  WorkingRole nvarchar(200),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  AdminRole nvarchar(300),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Team nvarchar(300),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RegistrationDate datetime2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  LastLogin datetime2,</t>
+  </si>
+  <si>
+    <t>create table Roles(</t>
+  </si>
+  <si>
+    <t>create table UserRoles(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Id nvarchar(100) primary key not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Id nvarchar(100) primary key not null, </t>
+  </si>
+  <si>
+    <t>create table Teams (</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Id int primary key not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Name] nvarchar(max),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  UserId nvarchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RoleId nvarchar(100) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [Name] nvarchar(500) not null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  UserName nvarchar(500) not null,</t>
   </si>
 </sst>
 </file>
@@ -6014,7 +6078,7 @@
   <dimension ref="A1:B206"/>
   <sheetViews>
     <sheetView topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204"/>
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7133,6 +7197,146 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8564D72-9AD0-4906-A5F8-3DCBB1B32BC7}">
+  <dimension ref="A1:A28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A1:A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>697</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD447"/>
   <sheetViews>
@@ -9819,7 +10023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
@@ -10133,8 +10337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10665,10 +10869,10 @@
         <v>24</v>
       </c>
       <c r="E29" s="75" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F29" s="76" t="s">
         <v>1136</v>
-      </c>
-      <c r="F29" s="76" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">

</xml_diff>